<commit_message>
Update for the Wk on excel only
</commit_message>
<xml_diff>
--- a/Matlab/ISO2631.xlsx
+++ b/Matlab/ISO2631.xlsx
@@ -375,8 +375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>